<commit_message>
16nov folder- silicon cover and menstrual cups updated
</commit_message>
<xml_diff>
--- a/daraz produts tracking/16-Nov-21/food silicon cover.xlsx
+++ b/daraz produts tracking/16-Nov-21/food silicon cover.xlsx
@@ -8,9 +8,10 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1_2(Nov 19)" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="64">
   <si>
     <t xml:space="preserve">DARAZ</t>
   </si>
@@ -75,121 +76,145 @@
     <t xml:space="preserve">5 months</t>
   </si>
   <si>
+    <t xml:space="preserve">View-source:https://www.daraz.pk/products/frakin-6pcs-universal-food-silicone-cover-silicone-stretch-lids-for-cookware-reusable-stretch-lids-silicone-lid-covers-silicone-lids-i217834964-s1428516162.html?spm=a2a0e.searchlist.list.1.60cd34a2MV2pa0&amp;search=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 months</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View-source:https://www.daraz.pk/products/6pcs-universal-food-silicone-cover-silicone-stretch-lids-for-cookware-reusable-stretch-lids-silicone-lid-covers-silicone-lids-i171066031-s1341406010.html?spm=a2a0e.searchlist.list.4.60cd34a2MV2pa0&amp;search=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 months</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View-source:https://www.daraz.pk/products/silicon-lids-cover-silicon-stretch-lids-universal-silicone-stretch-lids-for-food-preservation-flexible-silicone-bowl-covers-6pcs-universal-reusable-silicon-lids-wraps-for-bowls-cans-cookware-vacuum-food-storage-and-food-preservation-i217662955-s1450495914.html?spm=a2a0e.searchlist.list.8.60cd34a2MV2pa0&amp;search=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View-source:https://www.daraz.pk/products/6pcs-universal-food-silicone-cover-silicone-stretch-lids-for-cookware-reusable-stretch-lids-silicone-lid-covers-silicone-lids-i207952372-s1425518151.html?spm=a2a0e.searchlist.list.13.60cd34a2MV2pa0&amp;search=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 months</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View-source:https://www.daraz.pk/products/reusable-and-durable-pack-of-6-universal-stretch-seal-lid-silicone-lids-storage-covers-for-cookware-dish-covers-i209488087-s1415914563.html?spm=a2a0e.searchlist.list.23.60cd34a2MV2pa0&amp;search=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 months</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View-source:https://www.daraz.pk/products/universal-food-silicone-cover-lids-6-pack-flexible-silicone-bowl-covers-for-bowl-jar-glassware-kitchen-i133788653-s1294191686.html?spm=a2a0e.searchlist.list.26.60cd34a2MV2pa0&amp;search=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 months</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View-source:https://www.daraz.pk/products/6pcs-kitchen-reusable-silicone-seal-lid-universal-silicone-stretch-lids-for-food-preservation-vacuum-food-storage-bowl-cover-and-cookware-cover-for-kitchen-and-home-i195232429-s1419480649.html?spm=a2a0e.searchlist.list.29.60cd34a2MV2pa0&amp;search=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View-source:https://www.daraz.pk/products/6-pcs-kitchen-reusable-silicone-stretch-seal-lid-preservation-vacuum-food-storage-bowl-cover-i133796364-s1426347649.html?spm=a2a0e.searchlist.list.32.60cd34a2MV2pa0&amp;search=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily avg.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top 10 Sellers 6 days Avg.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top Seller Daily Avg.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAUNCH BUDGET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inventory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRODUCT NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inventory Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">units/day, 30 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Best Selling Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sourcing Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bleeding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daraz Comission Best Selling Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bleeding Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">units/day, 10 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delivery charges within City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daraz Comission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flyer Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reff Fee 1.25%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Profit per unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.daraz.pk/products/frakin-6pcs-universal-food-silicone-cover-silicone-stretch-lids-for-cookware-reusable-stretch-lids-silicone-lid-covers-silicone-lids-i217834964-s1428516162.html?spm=a2a0e.searchlist.list.1.60cd34a2MV2pa0&amp;search=1</t>
   </si>
   <si>
-    <t xml:space="preserve">14 months</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.daraz.pk/products/6pcs-universal-food-silicone-cover-silicone-stretch-lids-for-cookware-reusable-stretch-lids-silicone-lid-covers-silicone-lids-i171066031-s1341406010.html?spm=a2a0e.searchlist.list.4.60cd34a2MV2pa0&amp;search=1</t>
   </si>
   <si>
-    <t xml:space="preserve">6 months</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.daraz.pk/products/silicon-lids-cover-silicon-stretch-lids-universal-silicone-stretch-lids-for-food-preservation-flexible-silicone-bowl-covers-6pcs-universal-reusable-silicon-lids-wraps-for-bowls-cans-cookware-vacuum-food-storage-and-food-preservation-i217662955-s1450495914.html?spm=a2a0e.searchlist.list.8.60cd34a2MV2pa0&amp;search=1</t>
   </si>
   <si>
-    <t xml:space="preserve">7 month</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.daraz.pk/products/6pcs-universal-food-silicone-cover-silicone-stretch-lids-for-cookware-reusable-stretch-lids-silicone-lid-covers-silicone-lids-i207952372-s1425518151.html?spm=a2a0e.searchlist.list.13.60cd34a2MV2pa0&amp;search=1</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.daraz.pk/products/6pcs-universal-food-silicone-cover-silicone-stretch-lids-for-cookware-reusable-stretch-lids-silicone-lid-covers-silicone-lids-i207928693-s1412960520.html?spm=a2a0e.searchlist.list.20.60cd34a2MV2pa0&amp;search=1</t>
   </si>
   <si>
-    <t xml:space="preserve">8 months</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.daraz.pk/products/reusable-and-durable-pack-of-6-universal-stretch-seal-lid-silicone-lids-storage-covers-for-cookware-dish-covers-i209488087-s1415914563.html?spm=a2a0e.searchlist.list.23.60cd34a2MV2pa0&amp;search=1</t>
   </si>
   <si>
-    <t xml:space="preserve">7 months</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.daraz.pk/products/universal-food-silicone-cover-lids-6-pack-flexible-silicone-bowl-covers-for-bowl-jar-glassware-kitchen-i133788653-s1294191686.html?spm=a2a0e.searchlist.list.26.60cd34a2MV2pa0&amp;search=1</t>
   </si>
   <si>
-    <t xml:space="preserve">10 months</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.daraz.pk/products/6pcs-kitchen-reusable-silicone-seal-lid-universal-silicone-stretch-lids-for-food-preservation-vacuum-food-storage-bowl-cover-and-cookware-cover-for-kitchen-and-home-i195232429-s1419480649.html?spm=a2a0e.searchlist.list.29.60cd34a2MV2pa0&amp;search=1</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.daraz.pk/products/6-pcs-kitchen-reusable-silicone-stretch-seal-lid-preservation-vacuum-food-storage-bowl-cover-i133796364-s1426347649.html?spm=a2a0e.searchlist.list.32.60cd34a2MV2pa0&amp;search=1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily avg.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Top 10 Sellers 6 days Avg.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Top Seller Daily Avg.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAUNCH BUDGET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inventory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">units</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRODUCT NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inventory Cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">units/day, 30 days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Best Selling Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sourcing Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bleeding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daraz Comission Best Selling Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bleeding Cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">units/day, 10 days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delivery charges within City</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daraz Comission</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flyer Cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reff Fee 1.25%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Profit per unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">%</t>
   </si>
 </sst>
 </file>
@@ -873,8 +898,8 @@
   </sheetPr>
   <dimension ref="A1:BE61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -994,7 +1019,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="14" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
       <c r="B8" s="10" t="s">
         <v>15</v>
@@ -1020,7 +1045,9 @@
       <c r="I8" s="10" t="n">
         <v>1375</v>
       </c>
-      <c r="J8" s="10"/>
+      <c r="J8" s="10" t="n">
+        <v>1359</v>
+      </c>
       <c r="K8" s="10"/>
       <c r="L8" s="11"/>
       <c r="M8" s="5"/>
@@ -1074,7 +1101,7 @@
       <c r="BD8" s="1"/>
       <c r="BE8" s="1"/>
     </row>
-    <row r="9" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="14" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
       <c r="B9" s="14" t="s">
         <v>15</v>
@@ -1099,6 +1126,9 @@
       </c>
       <c r="I9" s="14" t="n">
         <v>3</v>
+      </c>
+      <c r="J9" s="14" t="n">
+        <v>0</v>
       </c>
       <c r="L9" s="15"/>
       <c r="M9" s="5"/>
@@ -1171,6 +1201,9 @@
       <c r="I10" s="14" t="n">
         <v>154</v>
       </c>
+      <c r="J10" s="14" t="n">
+        <v>145</v>
+      </c>
       <c r="L10" s="15"/>
       <c r="M10" s="5"/>
       <c r="N10" s="16"/>
@@ -1216,7 +1249,7 @@
       <c r="BD10" s="1"/>
       <c r="BE10" s="1"/>
     </row>
-    <row r="11" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="14" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1"/>
       <c r="B11" s="14" t="s">
         <v>15</v>
@@ -1241,6 +1274,9 @@
       </c>
       <c r="I11" s="14" t="n">
         <v>954</v>
+      </c>
+      <c r="J11" s="14" t="n">
+        <v>947</v>
       </c>
       <c r="L11" s="15"/>
       <c r="M11" s="5"/>
@@ -1287,7 +1323,7 @@
       <c r="BD11" s="1"/>
       <c r="BE11" s="1"/>
     </row>
-    <row r="12" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" s="14" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
       <c r="B12" s="14" t="s">
         <v>15</v>
@@ -1312,13 +1348,16 @@
       </c>
       <c r="I12" s="14" t="n">
         <v>1400</v>
+      </c>
+      <c r="J12" s="14" t="n">
+        <v>0</v>
       </c>
       <c r="L12" s="15"/>
       <c r="M12" s="5"/>
       <c r="N12" s="16"/>
       <c r="S12" s="15"/>
       <c r="T12" s="13" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
@@ -1358,7 +1397,7 @@
       <c r="BD12" s="1"/>
       <c r="BE12" s="1"/>
     </row>
-    <row r="13" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" s="14" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
       <c r="B13" s="14" t="s">
         <v>15</v>
@@ -1370,7 +1409,7 @@
         <v>177</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F13" s="14" t="n">
         <v>81</v>
@@ -1383,13 +1422,16 @@
       </c>
       <c r="I13" s="14" t="n">
         <v>20</v>
+      </c>
+      <c r="J13" s="14" t="n">
+        <v>19</v>
       </c>
       <c r="L13" s="15"/>
       <c r="M13" s="5"/>
       <c r="N13" s="16"/>
       <c r="S13" s="15"/>
       <c r="T13" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
@@ -1429,7 +1471,7 @@
       <c r="BD13" s="1"/>
       <c r="BE13" s="1"/>
     </row>
-    <row r="14" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="14" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
       <c r="B14" s="14" t="s">
         <v>15</v>
@@ -1441,7 +1483,7 @@
         <v>178</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F14" s="14" t="n">
         <v>68</v>
@@ -1454,13 +1496,16 @@
       </c>
       <c r="I14" s="14" t="n">
         <v>1360</v>
+      </c>
+      <c r="J14" s="14" t="n">
+        <v>1358</v>
       </c>
       <c r="L14" s="15"/>
       <c r="M14" s="5"/>
       <c r="N14" s="16"/>
       <c r="S14" s="15"/>
       <c r="T14" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
@@ -1500,7 +1545,7 @@
       <c r="BD14" s="1"/>
       <c r="BE14" s="1"/>
     </row>
-    <row r="15" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1"/>
       <c r="B15" s="14" t="s">
         <v>15</v>
@@ -1512,7 +1557,7 @@
         <v>200</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15" s="14" t="n">
         <v>351</v>
@@ -1525,13 +1570,16 @@
       </c>
       <c r="I15" s="14" t="n">
         <v>59</v>
+      </c>
+      <c r="J15" s="14" t="n">
+        <v>58</v>
       </c>
       <c r="L15" s="15"/>
       <c r="M15" s="5"/>
       <c r="N15" s="16"/>
       <c r="S15" s="15"/>
       <c r="T15" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
@@ -1571,7 +1619,7 @@
       <c r="BD15" s="1"/>
       <c r="BE15" s="1"/>
     </row>
-    <row r="16" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" s="14" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1"/>
       <c r="B16" s="14" t="s">
         <v>15</v>
@@ -1583,7 +1631,7 @@
         <v>184</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F16" s="14" t="n">
         <v>154</v>
@@ -1596,13 +1644,16 @@
       </c>
       <c r="I16" s="14" t="n">
         <v>14</v>
+      </c>
+      <c r="J16" s="14" t="n">
+        <v>10</v>
       </c>
       <c r="L16" s="15"/>
       <c r="M16" s="5"/>
       <c r="N16" s="16"/>
       <c r="S16" s="15"/>
       <c r="T16" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
@@ -1689,12 +1740,12 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J18" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K18" s="19"/>
       <c r="L18" s="19"/>
       <c r="M18" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N18" s="20" t="e">
         <f aca="false">AVERAGE(N8:N17)</f>
@@ -1723,12 +1774,12 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J19" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K19" s="22"/>
       <c r="L19" s="22"/>
       <c r="M19" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N19" s="23" t="e">
         <f aca="false">AVERAGE(N18:S18)</f>
@@ -1739,12 +1790,12 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J20" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K20" s="25"/>
       <c r="L20" s="25"/>
       <c r="M20" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N20" s="26" t="n">
         <f aca="false">AVERAGE(N8:S8)</f>
@@ -1761,7 +1812,7 @@
     <row r="23" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N24" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O24" s="29"/>
       <c r="P24" s="29"/>
@@ -1774,35 +1825,35 @@
       <c r="H25" s="30"/>
       <c r="I25" s="30"/>
       <c r="N25" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O25" s="31"/>
       <c r="P25" s="31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D26" s="32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E26" s="32"/>
       <c r="F26" s="32"/>
       <c r="G26" s="33"/>
       <c r="H26" s="32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I26" s="32"/>
       <c r="N26" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O26" s="34"/>
       <c r="P26" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D27" s="35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E27" s="36"/>
       <c r="F27" s="36" t="n">
@@ -1810,22 +1861,22 @@
       </c>
       <c r="G27" s="37"/>
       <c r="H27" s="38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I27" s="38" t="n">
         <v>45</v>
       </c>
       <c r="N27" s="34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O27" s="34"/>
       <c r="P27" s="34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D28" s="39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E28" s="39"/>
       <c r="F28" s="40" t="n">
@@ -1836,16 +1887,16 @@
       <c r="H28" s="41"/>
       <c r="I28" s="41"/>
       <c r="N28" s="34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O28" s="34"/>
       <c r="P28" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D29" s="39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E29" s="39"/>
       <c r="F29" s="40" t="n">
@@ -1853,7 +1904,7 @@
       </c>
       <c r="G29" s="37"/>
       <c r="H29" s="41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I29" s="41" t="n">
         <v>3.4</v>
@@ -1861,7 +1912,7 @@
     </row>
     <row r="30" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D30" s="40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E30" s="42"/>
       <c r="F30" s="40" t="n">
@@ -1871,7 +1922,7 @@
     </row>
     <row r="31" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D31" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E31" s="40"/>
       <c r="F31" s="40" t="n">
@@ -1881,7 +1932,7 @@
     </row>
     <row r="32" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D32" s="40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E32" s="40"/>
       <c r="F32" s="40" t="n">
@@ -1891,7 +1942,7 @@
     </row>
     <row r="33" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D33" s="40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E33" s="40"/>
       <c r="F33" s="40" t="n">
@@ -1901,7 +1952,7 @@
     </row>
     <row r="34" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D34" s="40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E34" s="40"/>
       <c r="F34" s="40" t="n">
@@ -1913,7 +1964,1119 @@
         <v>37.1393333333333</v>
       </c>
       <c r="H34" s="43" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="56" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="58" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="59" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="60" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="61" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="G5:R5"/>
+    <mergeCell ref="G6:L6"/>
+    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="T8" r:id="rId1" display="https://www.daraz.pk/products/frakin-6pcs-universal-food-silicone-cover-silicone-stretch-lids-for-cookware-reusable-stretch-lids-silicone-lid-covers-silicone-lids-i217834964-s1428516162.html?spm=a2a0e.searchlist.list.1.60cd34a2MV2pa0&amp;search=1"/>
+    <hyperlink ref="T9" r:id="rId2" display="https://www.daraz.pk/products/6pcs-universal-food-silicone-cover-silicone-stretch-lids-for-cookware-reusable-stretch-lids-silicone-lid-covers-silicone-lids-i171066031-s1341406010.html?spm=a2a0e.searchlist.list.4.60cd34a2MV2pa0&amp;search=1"/>
+    <hyperlink ref="T11" r:id="rId3" display="https://www.daraz.pk/products/6pcs-universal-food-silicone-cover-silicone-stretch-lids-for-cookware-reusable-stretch-lids-silicone-lid-covers-silicone-lids-i207952372-s1425518151.html?spm=a2a0e.searchlist.list.13.60cd34a2MV2pa0&amp;search=1"/>
+    <hyperlink ref="T12" r:id="rId4" display="https://www.daraz.pk/products/6pcs-universal-food-silicone-cover-silicone-stretch-lids-for-cookware-reusable-stretch-lids-silicone-lid-covers-silicone-lids-i171066031-s1341406010.html?spm=a2a0e.searchlist.list.4.60cd34a2MV2pa0&amp;search=1"/>
+    <hyperlink ref="T13" r:id="rId5" display="https://www.daraz.pk/products/reusable-and-durable-pack-of-6-universal-stretch-seal-lid-silicone-lids-storage-covers-for-cookware-dish-covers-i209488087-s1415914563.html?spm=a2a0e.searchlist.list.23.60cd34a2MV2pa0&amp;search=1"/>
+    <hyperlink ref="T14" r:id="rId6" display="https://www.daraz.pk/products/universal-food-silicone-cover-lids-6-pack-flexible-silicone-bowl-covers-for-bowl-jar-glassware-kitchen-i133788653-s1294191686.html?spm=a2a0e.searchlist.list.26.60cd34a2MV2pa0&amp;search=1"/>
+    <hyperlink ref="T16" r:id="rId7" display="https://www.daraz.pk/products/6-pcs-kitchen-reusable-silicone-stretch-seal-lid-preservation-vacuum-food-storage-bowl-cover-i133796364-s1426347649.html?spm=a2a0e.searchlist.list.32.60cd34a2MV2pa0&amp;search=1"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:BE61"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T8" activeCellId="0" sqref="T8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="18.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="17" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="28"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="21" style="1" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="23.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+    </row>
+    <row r="7" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="8"/>
+      <c r="N7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="R7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="S7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T7" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1"/>
+      <c r="B8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="10" t="n">
+        <v>186</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="10" t="n">
+        <v>83</v>
+      </c>
+      <c r="G8" s="10" t="n">
+        <v>1423</v>
+      </c>
+      <c r="H8" s="10" t="n">
+        <v>1389</v>
+      </c>
+      <c r="I8" s="10" t="n">
+        <v>1375</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="11" t="n">
+        <f aca="false">SUM(L8-M8)</f>
+        <v>0</v>
+      </c>
+      <c r="T8" s="13" t="s">
         <v>55</v>
+      </c>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+      <c r="AI8" s="1"/>
+      <c r="AJ8" s="1"/>
+      <c r="AK8" s="1"/>
+      <c r="AL8" s="1"/>
+      <c r="AM8" s="1"/>
+      <c r="AN8" s="1"/>
+      <c r="AO8" s="1"/>
+      <c r="AP8" s="1"/>
+      <c r="AQ8" s="1"/>
+      <c r="AR8" s="1"/>
+      <c r="AS8" s="1"/>
+      <c r="AT8" s="1"/>
+      <c r="AU8" s="1"/>
+      <c r="AV8" s="1"/>
+      <c r="AW8" s="1"/>
+      <c r="AX8" s="1"/>
+      <c r="AY8" s="1"/>
+      <c r="AZ8" s="1"/>
+      <c r="BA8" s="1"/>
+      <c r="BB8" s="1"/>
+      <c r="BC8" s="1"/>
+      <c r="BD8" s="1"/>
+      <c r="BE8" s="1"/>
+    </row>
+    <row r="9" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+      <c r="B9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" s="14" t="n">
+        <v>212</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="14" t="n">
+        <v>617</v>
+      </c>
+      <c r="G9" s="14" t="n">
+        <v>26</v>
+      </c>
+      <c r="H9" s="14" t="n">
+        <v>14</v>
+      </c>
+      <c r="I9" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="L9" s="15"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="16"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="1"/>
+      <c r="AG9" s="1"/>
+      <c r="AH9" s="1"/>
+      <c r="AI9" s="1"/>
+      <c r="AJ9" s="1"/>
+      <c r="AK9" s="1"/>
+      <c r="AL9" s="1"/>
+      <c r="AM9" s="1"/>
+      <c r="AN9" s="1"/>
+      <c r="AO9" s="1"/>
+      <c r="AP9" s="1"/>
+      <c r="AQ9" s="1"/>
+      <c r="AR9" s="1"/>
+      <c r="AS9" s="1"/>
+      <c r="AT9" s="1"/>
+      <c r="AU9" s="1"/>
+      <c r="AV9" s="1"/>
+      <c r="AW9" s="1"/>
+      <c r="AX9" s="1"/>
+      <c r="AY9" s="1"/>
+      <c r="AZ9" s="1"/>
+      <c r="BA9" s="1"/>
+      <c r="BB9" s="1"/>
+      <c r="BC9" s="1"/>
+      <c r="BD9" s="1"/>
+      <c r="BE9" s="1"/>
+    </row>
+    <row r="10" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+      <c r="B10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" s="14" t="n">
+        <v>167</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="14" t="n">
+        <v>142</v>
+      </c>
+      <c r="G10" s="14" t="n">
+        <v>163</v>
+      </c>
+      <c r="H10" s="14" t="n">
+        <v>146</v>
+      </c>
+      <c r="I10" s="14" t="n">
+        <v>154</v>
+      </c>
+      <c r="L10" s="15"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="16"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="1"/>
+      <c r="AJ10" s="1"/>
+      <c r="AK10" s="1"/>
+      <c r="AL10" s="1"/>
+      <c r="AM10" s="1"/>
+      <c r="AN10" s="1"/>
+      <c r="AO10" s="1"/>
+      <c r="AP10" s="1"/>
+      <c r="AQ10" s="1"/>
+      <c r="AR10" s="1"/>
+      <c r="AS10" s="1"/>
+      <c r="AT10" s="1"/>
+      <c r="AU10" s="1"/>
+      <c r="AV10" s="1"/>
+      <c r="AW10" s="1"/>
+      <c r="AX10" s="1"/>
+      <c r="AY10" s="1"/>
+      <c r="AZ10" s="1"/>
+      <c r="BA10" s="1"/>
+      <c r="BB10" s="1"/>
+      <c r="BC10" s="1"/>
+      <c r="BD10" s="1"/>
+      <c r="BE10" s="1"/>
+    </row>
+    <row r="11" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="B11" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="14" t="n">
+        <v>4</v>
+      </c>
+      <c r="D11" s="14" t="n">
+        <v>177</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="14" t="n">
+        <v>329</v>
+      </c>
+      <c r="G11" s="14" t="n">
+        <v>1009</v>
+      </c>
+      <c r="H11" s="14" t="n">
+        <v>973</v>
+      </c>
+      <c r="I11" s="14" t="n">
+        <v>954</v>
+      </c>
+      <c r="L11" s="15"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="16"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="1"/>
+      <c r="AH11" s="1"/>
+      <c r="AI11" s="1"/>
+      <c r="AJ11" s="1"/>
+      <c r="AK11" s="1"/>
+      <c r="AL11" s="1"/>
+      <c r="AM11" s="1"/>
+      <c r="AN11" s="1"/>
+      <c r="AO11" s="1"/>
+      <c r="AP11" s="1"/>
+      <c r="AQ11" s="1"/>
+      <c r="AR11" s="1"/>
+      <c r="AS11" s="1"/>
+      <c r="AT11" s="1"/>
+      <c r="AU11" s="1"/>
+      <c r="AV11" s="1"/>
+      <c r="AW11" s="1"/>
+      <c r="AX11" s="1"/>
+      <c r="AY11" s="1"/>
+      <c r="AZ11" s="1"/>
+      <c r="BA11" s="1"/>
+      <c r="BB11" s="1"/>
+      <c r="BC11" s="1"/>
+      <c r="BD11" s="1"/>
+      <c r="BE11" s="1"/>
+    </row>
+    <row r="12" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+      <c r="B12" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="D12" s="14" t="n">
+        <v>198</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="14" t="n">
+        <v>44</v>
+      </c>
+      <c r="G12" s="14" t="n">
+        <v>1402</v>
+      </c>
+      <c r="H12" s="14" t="n">
+        <v>1402</v>
+      </c>
+      <c r="I12" s="14" t="n">
+        <v>1400</v>
+      </c>
+      <c r="L12" s="15"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="16"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="1"/>
+      <c r="AH12" s="1"/>
+      <c r="AI12" s="1"/>
+      <c r="AJ12" s="1"/>
+      <c r="AK12" s="1"/>
+      <c r="AL12" s="1"/>
+      <c r="AM12" s="1"/>
+      <c r="AN12" s="1"/>
+      <c r="AO12" s="1"/>
+      <c r="AP12" s="1"/>
+      <c r="AQ12" s="1"/>
+      <c r="AR12" s="1"/>
+      <c r="AS12" s="1"/>
+      <c r="AT12" s="1"/>
+      <c r="AU12" s="1"/>
+      <c r="AV12" s="1"/>
+      <c r="AW12" s="1"/>
+      <c r="AX12" s="1"/>
+      <c r="AY12" s="1"/>
+      <c r="AZ12" s="1"/>
+      <c r="BA12" s="1"/>
+      <c r="BB12" s="1"/>
+      <c r="BC12" s="1"/>
+      <c r="BD12" s="1"/>
+      <c r="BE12" s="1"/>
+    </row>
+    <row r="13" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+      <c r="B13" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="14" t="n">
+        <v>7</v>
+      </c>
+      <c r="D13" s="14" t="n">
+        <v>177</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="14" t="n">
+        <v>81</v>
+      </c>
+      <c r="G13" s="14" t="n">
+        <v>21</v>
+      </c>
+      <c r="H13" s="14" t="n">
+        <v>20</v>
+      </c>
+      <c r="I13" s="14" t="n">
+        <v>20</v>
+      </c>
+      <c r="L13" s="15"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="16"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="1"/>
+      <c r="AE13" s="1"/>
+      <c r="AF13" s="1"/>
+      <c r="AG13" s="1"/>
+      <c r="AH13" s="1"/>
+      <c r="AI13" s="1"/>
+      <c r="AJ13" s="1"/>
+      <c r="AK13" s="1"/>
+      <c r="AL13" s="1"/>
+      <c r="AM13" s="1"/>
+      <c r="AN13" s="1"/>
+      <c r="AO13" s="1"/>
+      <c r="AP13" s="1"/>
+      <c r="AQ13" s="1"/>
+      <c r="AR13" s="1"/>
+      <c r="AS13" s="1"/>
+      <c r="AT13" s="1"/>
+      <c r="AU13" s="1"/>
+      <c r="AV13" s="1"/>
+      <c r="AW13" s="1"/>
+      <c r="AX13" s="1"/>
+      <c r="AY13" s="1"/>
+      <c r="AZ13" s="1"/>
+      <c r="BA13" s="1"/>
+      <c r="BB13" s="1"/>
+      <c r="BC13" s="1"/>
+      <c r="BD13" s="1"/>
+      <c r="BE13" s="1"/>
+    </row>
+    <row r="14" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="14" t="n">
+        <v>8</v>
+      </c>
+      <c r="D14" s="14" t="n">
+        <v>178</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="14" t="n">
+        <v>68</v>
+      </c>
+      <c r="G14" s="14" t="n">
+        <v>1362</v>
+      </c>
+      <c r="H14" s="14" t="n">
+        <v>1361</v>
+      </c>
+      <c r="I14" s="14" t="n">
+        <v>1360</v>
+      </c>
+      <c r="L14" s="15"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="16"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="1"/>
+      <c r="AG14" s="1"/>
+      <c r="AH14" s="1"/>
+      <c r="AI14" s="1"/>
+      <c r="AJ14" s="1"/>
+      <c r="AK14" s="1"/>
+      <c r="AL14" s="1"/>
+      <c r="AM14" s="1"/>
+      <c r="AN14" s="1"/>
+      <c r="AO14" s="1"/>
+      <c r="AP14" s="1"/>
+      <c r="AQ14" s="1"/>
+      <c r="AR14" s="1"/>
+      <c r="AS14" s="1"/>
+      <c r="AT14" s="1"/>
+      <c r="AU14" s="1"/>
+      <c r="AV14" s="1"/>
+      <c r="AW14" s="1"/>
+      <c r="AX14" s="1"/>
+      <c r="AY14" s="1"/>
+      <c r="AZ14" s="1"/>
+      <c r="BA14" s="1"/>
+      <c r="BB14" s="1"/>
+      <c r="BC14" s="1"/>
+      <c r="BD14" s="1"/>
+      <c r="BE14" s="1"/>
+    </row>
+    <row r="15" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1"/>
+      <c r="B15" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="14" t="n">
+        <v>9</v>
+      </c>
+      <c r="D15" s="14" t="n">
+        <v>200</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="14" t="n">
+        <v>351</v>
+      </c>
+      <c r="G15" s="14" t="n">
+        <v>60</v>
+      </c>
+      <c r="H15" s="14" t="n">
+        <v>59</v>
+      </c>
+      <c r="I15" s="14" t="n">
+        <v>59</v>
+      </c>
+      <c r="L15" s="15"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="16"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1"/>
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1"/>
+      <c r="AI15" s="1"/>
+      <c r="AJ15" s="1"/>
+      <c r="AK15" s="1"/>
+      <c r="AL15" s="1"/>
+      <c r="AM15" s="1"/>
+      <c r="AN15" s="1"/>
+      <c r="AO15" s="1"/>
+      <c r="AP15" s="1"/>
+      <c r="AQ15" s="1"/>
+      <c r="AR15" s="1"/>
+      <c r="AS15" s="1"/>
+      <c r="AT15" s="1"/>
+      <c r="AU15" s="1"/>
+      <c r="AV15" s="1"/>
+      <c r="AW15" s="1"/>
+      <c r="AX15" s="1"/>
+      <c r="AY15" s="1"/>
+      <c r="AZ15" s="1"/>
+      <c r="BA15" s="1"/>
+      <c r="BB15" s="1"/>
+      <c r="BC15" s="1"/>
+      <c r="BD15" s="1"/>
+      <c r="BE15" s="1"/>
+    </row>
+    <row r="16" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1"/>
+      <c r="B16" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="14" t="n">
+        <v>10</v>
+      </c>
+      <c r="D16" s="14" t="n">
+        <v>184</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="14" t="n">
+        <v>154</v>
+      </c>
+      <c r="G16" s="14" t="n">
+        <v>16</v>
+      </c>
+      <c r="H16" s="14" t="n">
+        <v>14</v>
+      </c>
+      <c r="I16" s="14" t="n">
+        <v>14</v>
+      </c>
+      <c r="L16" s="15"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="16"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1"/>
+      <c r="AF16" s="1"/>
+      <c r="AG16" s="1"/>
+      <c r="AH16" s="1"/>
+      <c r="AI16" s="1"/>
+      <c r="AJ16" s="1"/>
+      <c r="AK16" s="1"/>
+      <c r="AL16" s="1"/>
+      <c r="AM16" s="1"/>
+      <c r="AN16" s="1"/>
+      <c r="AO16" s="1"/>
+      <c r="AP16" s="1"/>
+      <c r="AQ16" s="1"/>
+      <c r="AR16" s="1"/>
+      <c r="AS16" s="1"/>
+      <c r="AT16" s="1"/>
+      <c r="AU16" s="1"/>
+      <c r="AV16" s="1"/>
+      <c r="AW16" s="1"/>
+      <c r="AX16" s="1"/>
+      <c r="AY16" s="1"/>
+      <c r="AZ16" s="1"/>
+      <c r="BA16" s="1"/>
+      <c r="BB16" s="1"/>
+      <c r="BC16" s="1"/>
+      <c r="BD16" s="1"/>
+      <c r="BE16" s="1"/>
+    </row>
+    <row r="17" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="16"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="17"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="1"/>
+      <c r="AF17" s="1"/>
+      <c r="AG17" s="1"/>
+      <c r="AH17" s="1"/>
+      <c r="AI17" s="1"/>
+      <c r="AJ17" s="1"/>
+      <c r="AK17" s="1"/>
+      <c r="AL17" s="1"/>
+      <c r="AM17" s="1"/>
+      <c r="AN17" s="1"/>
+      <c r="AO17" s="1"/>
+      <c r="AP17" s="1"/>
+      <c r="AQ17" s="1"/>
+      <c r="AR17" s="1"/>
+      <c r="AS17" s="1"/>
+      <c r="AT17" s="1"/>
+      <c r="AU17" s="1"/>
+      <c r="AV17" s="1"/>
+      <c r="AW17" s="1"/>
+      <c r="AX17" s="1"/>
+      <c r="AY17" s="1"/>
+      <c r="AZ17" s="1"/>
+      <c r="BA17" s="1"/>
+      <c r="BB17" s="1"/>
+      <c r="BC17" s="1"/>
+      <c r="BD17" s="1"/>
+      <c r="BE17" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J18" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="N18" s="20" t="e">
+        <f aca="false">AVERAGE(N8:N17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O18" s="20" t="e">
+        <f aca="false">AVERAGE(O8:O17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P18" s="20" t="e">
+        <f aca="false">AVERAGE(P8:P17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q18" s="20" t="e">
+        <f aca="false">AVERAGE(Q8:Q17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R18" s="20" t="e">
+        <f aca="false">AVERAGE(R8:R17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S18" s="21" t="n">
+        <f aca="false">AVERAGE(S8:S17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J19" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="N19" s="23" t="e">
+        <f aca="false">AVERAGE(N18:S18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O19" s="23"/>
+      <c r="S19" s="24"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J20" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="N20" s="26" t="n">
+        <f aca="false">AVERAGE(N8:S8)</f>
+        <v>0</v>
+      </c>
+      <c r="O20" s="26"/>
+      <c r="P20" s="27"/>
+      <c r="Q20" s="27"/>
+      <c r="R20" s="27"/>
+      <c r="S20" s="28"/>
+    </row>
+    <row r="21" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N24" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="O24" s="29"/>
+      <c r="P24" s="29"/>
+    </row>
+    <row r="25" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="N25" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="O25" s="31"/>
+      <c r="P25" s="31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D26" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="I26" s="32"/>
+      <c r="N26" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="O26" s="34"/>
+      <c r="P26" s="34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D27" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36" t="n">
+        <v>105</v>
+      </c>
+      <c r="G27" s="37"/>
+      <c r="H27" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="I27" s="38" t="n">
+        <v>45</v>
+      </c>
+      <c r="N27" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="O27" s="34"/>
+      <c r="P27" s="34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D28" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="39"/>
+      <c r="F28" s="40" t="n">
+        <f aca="false">(F27/100)*I29</f>
+        <v>3.57</v>
+      </c>
+      <c r="G28" s="37"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="41"/>
+      <c r="N28" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="O28" s="34"/>
+      <c r="P28" s="34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D29" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="39"/>
+      <c r="F29" s="40" t="n">
+        <v>49</v>
+      </c>
+      <c r="G29" s="37"/>
+      <c r="H29" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="I29" s="41" t="n">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="30" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D30" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="42"/>
+      <c r="F30" s="40" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="G30" s="30"/>
+    </row>
+    <row r="31" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D31" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40" t="n">
+        <f aca="false">(F27*0.0125)</f>
+        <v>1.3125</v>
+      </c>
+    </row>
+    <row r="32" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D32" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40" t="n">
+        <f aca="false">(F28+F29+F31)*16%</f>
+        <v>8.6212</v>
+      </c>
+    </row>
+    <row r="33" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D33" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40" t="n">
+        <f aca="false">(I27+F28+F30+F31+F32)</f>
+        <v>66.0037</v>
+      </c>
+    </row>
+    <row r="34" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D34" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40" t="n">
+        <f aca="false">F27-F33</f>
+        <v>38.9963</v>
+      </c>
+      <c r="G34" s="1" t="n">
+        <f aca="false">(F34/F27)*100</f>
+        <v>37.1393333333333</v>
+      </c>
+      <c r="H34" s="43" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1978,7 +3141,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1989,7 +3152,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2001,7 +3164,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2012,7 +3175,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>